<commit_message>
Fixed title style in css and integrated p0036 from Mr.Vengadesan
</commit_message>
<xml_diff>
--- a/paramData Excels/P0036.xlsx
+++ b/paramData Excels/P0036.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>COLUMN_KEY</t>
   </si>
@@ -87,9 +87,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>SA</t>
-  </si>
-  <si>
     <t>float64</t>
   </si>
   <si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t>Sum Assured</t>
+  </si>
+  <si>
+    <t>NofInstalments</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>No Of Installments</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,15 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,16 +506,16 @@
     </row>
     <row r="2" spans="1:20">
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -517,13 +527,13 @@
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
       </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -531,24 +541,50 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
P0036 changed and excel updated
</commit_message>
<xml_diff>
--- a/paramData Excels/P0036.xlsx
+++ b/paramData Excels/P0036.xlsx
@@ -102,9 +102,6 @@
     <t>Sum Assured</t>
   </si>
   <si>
-    <t>NofInstalments</t>
-  </si>
-  <si>
     <t>Sa</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>No Of Installments</t>
+  </si>
+  <si>
+    <t>Noofinstalments</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,12 +432,12 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
@@ -512,22 +512,22 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
@@ -541,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>

</xml_diff>